<commit_message>
Fixed bug with schedule not being updaed/updated for all
</commit_message>
<xml_diff>
--- a/templates/filled_template.xlsx
+++ b/templates/filled_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neiman/Documents/Projects/Coding/nplcore/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94064EDB-A877-6949-B46C-DB3DF39999CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2A9F490-DB71-D647-8242-0973768D820D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1860" windowWidth="28040" windowHeight="17260" activeTab="2" xr2:uid="{88D35EFF-2385-9E4C-A9AE-1ECABB4945D7}"/>
+    <workbookView xWindow="780" yWindow="1860" windowWidth="28040" windowHeight="17260" activeTab="4" xr2:uid="{88D35EFF-2385-9E4C-A9AE-1ECABB4945D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Techs" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="67">
   <si>
     <t>Monday</t>
   </si>
@@ -551,12 +551,13 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{560EA112-EEEB-4549-AFA0-228DAA657276}" name="CustomModsTable" displayName="CustomModsTable" ref="A3:E4" totalsRowShown="0">
-  <autoFilter ref="A3:E4" xr:uid="{560EA112-EEEB-4549-AFA0-228DAA657276}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{560EA112-EEEB-4549-AFA0-228DAA657276}" name="CustomModsTable" displayName="CustomModsTable" ref="A3:F4" totalsRowShown="0">
+  <autoFilter ref="A3:F4" xr:uid="{560EA112-EEEB-4549-AFA0-228DAA657276}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{438C46B6-0993-5F49-8874-8162B699718F}" name="Section"/>
     <tableColumn id="2" xr3:uid="{9A88EC7A-E958-EB4B-B54B-09FB4E7C723B}" name="Instructor"/>
     <tableColumn id="3" xr3:uid="{BD1B8B4E-AD26-184E-9A9A-38494EC2D7C1}" name="Week"/>
+    <tableColumn id="6" xr3:uid="{6C05BB42-D465-1741-9554-8528F7086DBC}" name="Note"/>
     <tableColumn id="4" xr3:uid="{D12C408E-B189-9141-81E3-AEF9D0C7D7B7}" name="Time"/>
     <tableColumn id="5" xr3:uid="{928EF546-A412-D442-A344-E167ECF383FC}" name="Equipment"/>
   </tableColumns>
@@ -1270,7 +1271,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{923A556D-1123-1F43-A77A-46BDA673057C}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
@@ -1345,7 +1346,7 @@
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1445,10 +1446,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F056D647-2C2A-4240-8D5C-FF0F5D3E080D}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1456,7 +1457,7 @@
     <col min="2" max="2" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -1464,7 +1465,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1475,9 +1476,12 @@
         <v>17</v>
       </c>
       <c r="D3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" t="s">
         <v>62</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>